<commit_message>
refactor: added auto-properties for models, fixed ci and uploaded a new version of the schedule
</commit_message>
<xml_diff>
--- a/ScheduleParser/Расписание.xlsx
+++ b/ScheduleParser/Расписание.xlsx
@@ -280,7 +280,7 @@
     <t xml:space="preserve">ООО «НМТ — Новые мобильные технологии»</t>
   </si>
   <si>
-    <t xml:space="preserve">СП, бакалавры МОиАИС, ГЭК 5006-01</t>
+    <t xml:space="preserve">СП, бакалавры техпрога, ГЭК 5006-01</t>
   </si>
   <si>
     <t xml:space="preserve">Белошапкин Михаил Юрьевич</t>
@@ -347,7 +347,7 @@
     <t xml:space="preserve">11:00, ауд. 3381</t>
   </si>
   <si>
-    <t xml:space="preserve">ИАС, бакалавры МОиАИС, ГЭК 5006-02</t>
+    <t xml:space="preserve">ИАС, бакалавры техпрога, ГЭК 5006-02</t>
   </si>
   <si>
     <t xml:space="preserve">Власов Илья Максимович</t>
@@ -458,7 +458,7 @@
     <t xml:space="preserve">16:00, ауд. 3381</t>
   </si>
   <si>
-    <t xml:space="preserve">ИАС, бакалавры МОиАИС, ГЭК 5006-03</t>
+    <t xml:space="preserve">ИАС, бакалавры техпрога, ГЭК 5006-03</t>
   </si>
   <si>
     <t xml:space="preserve">Панарин Павел Михайлович</t>
@@ -554,7 +554,7 @@
     <t xml:space="preserve">29 мая (понедельник)</t>
   </si>
   <si>
-    <t xml:space="preserve">Информатика/ПА, бакалавры МОиАИС, ГЭК 5006-04</t>
+    <t xml:space="preserve">Информатика/ПА, бакалавры техпрога, ГЭК 5006-04</t>
   </si>
   <si>
     <t xml:space="preserve">Бабич Никита Викторович</t>
@@ -659,7 +659,7 @@
     <t xml:space="preserve">Косовская Татьяна Матвеевна</t>
   </si>
   <si>
-    <t xml:space="preserve">Информатика/ПА, бакалавры МОиАИС, ГЭК 5006-05</t>
+    <t xml:space="preserve">Информатика/ПА, бакалавры техпрога, ГЭК 5006-05</t>
   </si>
   <si>
     <t xml:space="preserve">Куликов Михаил Алексеевич</t>
@@ -728,7 +728,7 @@
     <t xml:space="preserve">17:00, ауд. 3381</t>
   </si>
   <si>
-    <t xml:space="preserve">Информатика/ПА, магистры МОиАИС, ГЭК 5665-02</t>
+    <t xml:space="preserve">Информатика/ПА, магистры техпрога, ГЭК 5665-02</t>
   </si>
   <si>
     <t xml:space="preserve">Архипов Иван Сергеевич</t>
@@ -958,7 +958,7 @@
     <t xml:space="preserve">7 июня (среда)</t>
   </si>
   <si>
-    <t xml:space="preserve">СП, магистры МОиАИС, ГЭК 5665-03</t>
+    <t xml:space="preserve">СП, магистры техпрога, ГЭК 5665-03</t>
   </si>
   <si>
     <t xml:space="preserve">Борисоглебская Елена Александровна</t>
@@ -1006,7 +1006,7 @@
     <t xml:space="preserve">9 июня (пятница)</t>
   </si>
   <si>
-    <t xml:space="preserve">СП, бакалавры МОиАИС, ГЭК 5006-06</t>
+    <t xml:space="preserve">СП, бакалавры техпрога, ГЭК 5006-06</t>
   </si>
   <si>
     <t xml:space="preserve">Вильданов Эмир Флоридович</t>
@@ -1084,7 +1084,7 @@
     <t xml:space="preserve">Анализ и классификация затрат людей на лекарственные препараты с использованием технологий машинного обучения</t>
   </si>
   <si>
-    <t xml:space="preserve">СП, бакалавры МОиАИС, ГЭК 5006-07</t>
+    <t xml:space="preserve">СП, бакалавры техпрога, ГЭК 5006-07</t>
   </si>
   <si>
     <t xml:space="preserve">Глушень Павел Владимирович</t>
@@ -1635,7 +1635,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Yurii Litvinov" id="{ADEC7136-ECFC-BE0A-95F9-35FF1FDC160C}" userId="459951580" providerId="Teamlab"/>
+  <person displayName="Yurii Litvinov" id="{6E0AB834-38E6-C8CC-05E0-ED9F599E1A93}" userId="459951580" providerId="Teamlab"/>
 </personList>
 </file>
 
@@ -2051,11 +2051,11 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="G93" dT="2023-04-02T14:53:28.31Z" personId="{ADEC7136-ECFC-BE0A-95F9-35FF1FDC160C}" id="{F8F392F9-6CA2-38A7-F62E-7EB58FC3356F}" done="0">
+  <threadedComment ref="G93" dT="2023-04-02T14:53:28.31Z" personId="{6E0AB834-38E6-C8CC-05E0-ED9F599E1A93}" id="{F8F392F9-6CA2-38A7-F62E-7EB58FC3356F}" done="0">
     <text xml:space="preserve">На 14:00
 </text>
   </threadedComment>
-  <threadedComment ref="G96" dT="2023-04-02T14:53:53.96Z" personId="{ADEC7136-ECFC-BE0A-95F9-35FF1FDC160C}" id="{EA695E15-C0E6-D2C6-98F7-B97DB90E8DB7}" done="0">
+  <threadedComment ref="G96" dT="2023-04-02T14:53:53.96Z" personId="{6E0AB834-38E6-C8CC-05E0-ED9F599E1A93}" id="{EA695E15-C0E6-D2C6-98F7-B97DB90E8DB7}" done="0">
     <text xml:space="preserve">На 10:00
 </text>
   </threadedComment>
@@ -2071,7 +2071,7 @@
   <sheetViews>
     <sheetView topLeftCell="A1" zoomScale="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.630000000000001" defaultRowHeight="15.75" customHeight="1"/>
@@ -2109,7 +2109,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" ht="25.5">
+    <row r="2" ht="24">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>6</v>
@@ -2125,7 +2125,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" ht="25.5">
+    <row r="3" ht="24">
       <c r="A3" s="2"/>
       <c r="B3" s="3" t="s">
         <v>9</v>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" ht="25.5">
+    <row r="4" ht="24">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" ht="25.5">
+    <row r="5" ht="24">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" ht="25.5">
+    <row r="6" ht="24">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" ht="25.5">
+    <row r="7" ht="24">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" ht="25.5">
+    <row r="8" ht="24">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" ht="25.5">
+    <row r="9" ht="24">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -2281,7 +2281,7 @@
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" ht="25.5">
+    <row r="10" ht="24">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -2301,7 +2301,7 @@
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
     </row>
-    <row r="11" ht="25.5">
+    <row r="11" ht="24">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -2321,7 +2321,7 @@
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
     </row>
-    <row r="12" ht="25.5">
+    <row r="12" ht="24">
       <c r="A12" s="7">
         <v>9</v>
       </c>
@@ -2377,7 +2377,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" ht="25.5">
+    <row r="16" ht="24">
       <c r="A16" s="7">
         <v>1</v>
       </c>
@@ -2408,7 +2408,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" ht="25.5">
+    <row r="18" ht="24">
       <c r="A18" s="7">
         <v>3</v>
       </c>
@@ -2428,7 +2428,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" ht="25.5">
+    <row r="19" ht="24">
       <c r="A19" s="7">
         <v>4</v>
       </c>
@@ -2458,7 +2458,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" ht="25.5">
+    <row r="21" ht="24">
       <c r="A21" s="2"/>
       <c r="B21" s="3" t="s">
         <v>67</v>
@@ -2474,7 +2474,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" ht="25.5">
+    <row r="22" ht="24">
       <c r="A22" s="2"/>
       <c r="B22" s="3" t="s">
         <v>9</v>
@@ -2490,7 +2490,7 @@
       </c>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" ht="25.5">
+    <row r="23" ht="24">
       <c r="A23" s="7">
         <v>1</v>
       </c>
@@ -2514,7 +2514,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" ht="38.25">
+    <row r="24" ht="36">
       <c r="A24" s="7">
         <v>2</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" ht="25.5">
+    <row r="25" ht="24">
       <c r="A25" s="7">
         <v>3</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" ht="25.5">
+    <row r="26" ht="24">
       <c r="A26" s="7">
         <v>4</v>
       </c>
@@ -2645,7 +2645,7 @@
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
     </row>
-    <row r="32" ht="25.5">
+    <row r="32" ht="24">
       <c r="A32" s="7"/>
       <c r="B32" s="3" t="s">
         <v>88</v>
@@ -2661,7 +2661,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" ht="25.5">
+    <row r="33" ht="24">
       <c r="A33" s="7"/>
       <c r="B33" s="3" t="s">
         <v>91</v>
@@ -2677,7 +2677,7 @@
       </c>
       <c r="H33" s="5"/>
     </row>
-    <row r="34" ht="25.5">
+    <row r="34" ht="24">
       <c r="A34" s="7">
         <v>1</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" ht="25.5">
+    <row r="35" ht="24">
       <c r="A35" s="7">
         <v>2</v>
       </c>
@@ -2725,7 +2725,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="36" ht="25.5">
+    <row r="36" ht="24">
       <c r="A36" s="7">
         <v>3</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" ht="25.5">
+    <row r="37" ht="24">
       <c r="A37" s="7">
         <v>4</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="38" ht="25.5">
+    <row r="38" ht="24">
       <c r="A38" s="7">
         <v>5</v>
       </c>
@@ -2793,7 +2793,7 @@
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
     </row>
-    <row r="39" ht="51">
+    <row r="39" ht="48">
       <c r="A39" s="7">
         <v>6</v>
       </c>
@@ -2812,7 +2812,7 @@
       <c r="F39" s="4"/>
       <c r="G39" s="10"/>
     </row>
-    <row r="40" ht="25.5">
+    <row r="40" ht="24">
       <c r="A40" s="7">
         <v>7</v>
       </c>
@@ -2829,7 +2829,7 @@
       <c r="F40" s="4"/>
       <c r="G40" s="10"/>
     </row>
-    <row r="41" ht="25.5">
+    <row r="41" ht="24">
       <c r="A41" s="7">
         <v>8</v>
       </c>
@@ -2848,7 +2848,7 @@
       <c r="F41" s="4"/>
       <c r="G41" s="10"/>
     </row>
-    <row r="42" ht="25.5">
+    <row r="42" ht="24">
       <c r="A42" s="7">
         <v>9</v>
       </c>
@@ -2867,7 +2867,7 @@
       <c r="F42" s="4"/>
       <c r="G42" s="10"/>
     </row>
-    <row r="43" ht="25.5">
+    <row r="43" ht="24">
       <c r="A43" s="7">
         <v>10</v>
       </c>
@@ -2904,7 +2904,7 @@
       <c r="F45" s="4"/>
       <c r="G45" s="10"/>
     </row>
-    <row r="46" ht="25.5">
+    <row r="46" ht="15.75">
       <c r="A46" s="7"/>
       <c r="B46" s="3" t="s">
         <v>127</v>
@@ -2917,7 +2917,7 @@
       <c r="F46" s="4"/>
       <c r="G46" s="10"/>
     </row>
-    <row r="47" ht="25.5">
+    <row r="47" ht="24">
       <c r="A47" s="7">
         <v>1</v>
       </c>
@@ -2936,7 +2936,7 @@
       <c r="F47" s="4"/>
       <c r="G47" s="10"/>
     </row>
-    <row r="48" ht="25.5">
+    <row r="48" ht="24">
       <c r="A48" s="7">
         <v>2</v>
       </c>
@@ -2955,7 +2955,7 @@
       <c r="F48" s="4"/>
       <c r="G48" s="10"/>
     </row>
-    <row r="49" ht="25.5">
+    <row r="49" ht="24">
       <c r="A49" s="7">
         <v>3</v>
       </c>
@@ -2974,7 +2974,7 @@
       <c r="F49" s="4"/>
       <c r="G49" s="10"/>
     </row>
-    <row r="50" ht="25.5">
+    <row r="50" ht="24">
       <c r="A50" s="7">
         <v>4</v>
       </c>
@@ -2993,7 +2993,7 @@
       <c r="F50" s="4"/>
       <c r="G50" s="10"/>
     </row>
-    <row r="51" ht="25.5">
+    <row r="51" ht="24">
       <c r="A51" s="7">
         <v>5</v>
       </c>
@@ -3012,7 +3012,7 @@
       <c r="F51" s="4"/>
       <c r="G51" s="10"/>
     </row>
-    <row r="52" ht="25.5">
+    <row r="52" ht="24">
       <c r="A52" s="7">
         <v>6</v>
       </c>
@@ -3031,7 +3031,7 @@
       <c r="F52" s="4"/>
       <c r="G52" s="10"/>
     </row>
-    <row r="53" ht="25.5">
+    <row r="53" ht="24">
       <c r="A53" s="7">
         <v>7</v>
       </c>
@@ -3050,7 +3050,7 @@
       <c r="F53" s="4"/>
       <c r="G53" s="10"/>
     </row>
-    <row r="54" ht="25.5">
+    <row r="54" ht="24">
       <c r="A54" s="7">
         <v>8</v>
       </c>
@@ -3069,7 +3069,7 @@
       <c r="F54" s="4"/>
       <c r="G54" s="10"/>
     </row>
-    <row r="55" ht="25.5">
+    <row r="55" ht="24">
       <c r="A55" s="7">
         <v>9</v>
       </c>
@@ -3088,7 +3088,7 @@
       <c r="F55" s="4"/>
       <c r="G55" s="10"/>
     </row>
-    <row r="56" ht="38.25">
+    <row r="56" ht="36">
       <c r="A56" s="7">
         <v>10</v>
       </c>
@@ -3107,7 +3107,7 @@
       <c r="F56" s="4"/>
       <c r="G56" s="10"/>
     </row>
-    <row r="57" ht="25.5">
+    <row r="57" ht="24">
       <c r="A57" s="7">
         <v>11</v>
       </c>
@@ -3136,7 +3136,7 @@
       <c r="G58" s="5"/>
       <c r="H58" s="5"/>
     </row>
-    <row r="59" ht="25.5">
+    <row r="59" ht="24">
       <c r="A59" s="2"/>
       <c r="B59" s="3" t="s">
         <v>159</v>
@@ -3152,7 +3152,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="60" ht="25.5">
+    <row r="60" ht="24">
       <c r="A60" s="2"/>
       <c r="B60" s="3" t="s">
         <v>9</v>
@@ -3168,7 +3168,7 @@
       </c>
       <c r="H60" s="5"/>
     </row>
-    <row r="61" ht="25.5">
+    <row r="61" ht="24">
       <c r="A61" s="7">
         <v>1</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="62" ht="38.25">
+    <row r="62" ht="36">
       <c r="A62" s="7">
         <v>2</v>
       </c>
@@ -3216,7 +3216,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="63" ht="25.5">
+    <row r="63" ht="24">
       <c r="A63" s="7">
         <v>3</v>
       </c>
@@ -3240,7 +3240,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="64" ht="38.25">
+    <row r="64" ht="36">
       <c r="A64" s="7">
         <v>4</v>
       </c>
@@ -3346,7 +3346,7 @@
       <c r="G69" s="6"/>
       <c r="H69" s="6"/>
     </row>
-    <row r="70">
+    <row r="70" ht="15.75">
       <c r="A70" s="7"/>
       <c r="B70" s="3" t="s">
         <v>54</v>
@@ -3521,7 +3521,7 @@
       <c r="F79" s="4"/>
       <c r="G79" s="5"/>
     </row>
-    <row r="80">
+    <row r="80" ht="15.75">
       <c r="A80" s="2"/>
       <c r="B80" s="3" t="s">
         <v>217</v>
@@ -4062,7 +4062,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" ht="24">
       <c r="A109" s="2"/>
       <c r="B109" s="3" t="s">
         <v>54</v>
@@ -4247,7 +4247,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="119">
+    <row r="119" ht="24">
       <c r="A119" s="2"/>
       <c r="B119" s="3" t="s">
         <v>9</v>
@@ -4479,7 +4479,7 @@
       <c r="G130" s="5"/>
       <c r="H130" s="5"/>
     </row>
-    <row r="131">
+    <row r="131" ht="15.75">
       <c r="A131" s="2"/>
       <c r="B131" s="3" t="s">
         <v>54</v>

</xml_diff>